<commit_message>
added feature to read query and dataelement from text file
</commit_message>
<xml_diff>
--- a/variants.xlsx
+++ b/variants.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A211"/>
+  <dimension ref="A1:A167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,1470 +443,1162 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>003961b5-bb60-41aa-8660-264dc00e642b</t>
+          <t>00791c93-b52b-404b-8174-af589b07ae9a</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>00cbc5ac-2516-4b8e-aa31-f91ceb022e00</t>
+          <t>0269322c-7cbb-410e-80f8-82cfbb526441</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>00da7bf5-bc31-43dd-bd5e-123e9bb3222e</t>
+          <t>03ce6d16-dfd6-4e3f-bb96-d1273811208e</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>025d2ec5-5720-4de3-bcff-dfce927f1f08</t>
+          <t>06541c8b-be7a-42bb-9c41-7c4f7c725d8b</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02e5cd4e-4aac-4eb5-849c-4ae59149efe5</t>
+          <t>0ab4d20a-5d2a-4f4e-8f60-94ae1bb4a54c</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04cb3cf5-6c02-4bc6-b201-1f5ed5787ccb</t>
+          <t>0af1db7d-242f-452e-8a0a-9abe10d151e5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0738da58-89b2-4e78-a25c-8d52ce60c113</t>
+          <t>0d88b27f-9718-4dd0-ac52-7170e9e9052b</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>075f21f2-d925-451e-a510-e98a86ece7b7</t>
+          <t>0e060eed-1bc4-4b91-9558-aedba0282534</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>07fef7a1-97a5-4160-bfdf-8f0984aa7ebd</t>
+          <t>0f781096-05af-46ed-a27e-94a389006aa7</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>084e3bac-d186-46ad-a534-1d694bb32ef9</t>
+          <t>10d00dbf-dd80-4878-b98c-21592e529a82</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>09396f93-64e9-4170-ba83-6ecead9618c4</t>
+          <t>1130fbaa-c3ba-42c7-a61e-92b6bf6f2649</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0bbb3047-3e35-446f-a1e9-f4b6350b2435</t>
+          <t>139dc2bb-90d6-420f-b1e2-dde845fa97c4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0c6a6c54-eb60-49b2-8e7f-4ef06565a6c4</t>
+          <t>13b796ec-e8c3-4b69-a0ed-d30ec9a6ff90</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0ca2ae0a-4d32-459b-a675-186c294a45a1</t>
+          <t>15d3003c-3faa-4a75-84cc-45e918ca0823</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0e34d546-efa8-43b5-8bb5-cfa50db39818</t>
+          <t>19961be1-2903-4aef-97be-03058d318929</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0e7662f1-5a74-4b14-bf3f-8398a9d5972b</t>
+          <t>19c1e2ba-1af5-4bbd-af5f-bd13a7a8e34f</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0ecc7fc5-61c9-4acf-b1f2-a5767f03171f</t>
+          <t>1a77887b-d0fd-4f8d-9335-80656ceca52a</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10a9b6a7-95a1-43eb-9cff-c77c1a8420d1</t>
+          <t>1d841aa0-44f7-4d1c-ae1a-d39275fb7ccc</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>11bd0fce-1c23-4142-b17d-481e871ab4d0</t>
+          <t>1d93cac8-6976-417c-9414-babee664118b</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>121e2126-6960-4801-881b-1343d56c62b5</t>
+          <t>1e4cf7ee-a218-47c2-9503-21ddb8b21807</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>12fa6d66-212d-4e63-bd15-15ffad38526c</t>
+          <t>2112ce42-3dde-41b4-b01d-a14f340a388b</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1302d799-3e1a-49ff-92b2-1c723381f597</t>
+          <t>2205d373-aed4-410c-b2d8-4d8703757620</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>13587a3b-c33d-4dac-acc5-a488d49ef697</t>
+          <t>22b58dc2-9d14-42ba-b830-5d25be58a2a6</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1638d022-abb1-4123-859e-23bb55172144</t>
+          <t>295ada5d-677d-4dee-9195-9416d077186b</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>17bef174-b9d4-45e7-bfad-ddb9793dd0d5</t>
+          <t>2a089712-cd39-47a6-a888-b2348aaf276a</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18060368-e01b-4572-94f0-e8514ab1577b</t>
+          <t>2a995c65-c4f3-4a3d-84e9-641fa2db780d</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18e308e1-0f1b-4e0a-a646-a7079eb52099</t>
+          <t>2fb3c587-c22a-4118-ae18-dd0289cc6c7a</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18f913d9-7715-4b81-a2ac-ca29a566d019</t>
+          <t>3257cae6-3eec-4688-8bf8-60c7514229cb</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>194fcd48-6a54-4614-9adc-8b5fe1740166</t>
+          <t>33a5c8c5-ab9d-4c67-9e52-d6e989c8908d</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>196f6ec4-556c-47d6-9ec2-4632be582aa5</t>
+          <t>34e9bb94-1473-4688-90a1-9274a3c8488a</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1d5e6408-584e-4e9a-b6fa-e0a64544bb2a</t>
+          <t>362c24fd-7dcf-4cd5-90ca-08764d1e3d62</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1da78358-62c3-4083-afe9-55b0357edda7</t>
+          <t>374f9918-2f82-4b87-b705-7f4a61d1d771</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1e8b1df2-3c2d-4407-8469-4ef7cb099911</t>
+          <t>3793a1eb-98e5-4524-9079-4ba7179b244b</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1f18d112-dcba-4941-bffb-2cece8dc36da</t>
+          <t>3908d03b-a2fd-4d67-9fe0-b34ca3087921</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>218a041e-67ff-4e4f-a973-de9c00c40870</t>
+          <t>3b2392ac-d781-4be5-bc25-d3958d48ec42</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>21e1982a-0c73-4307-9c61-b246b68ff5d9</t>
+          <t>3d89f48a-5583-4721-8bf9-09d2a7b6ca9f</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>22813a95-a215-4c40-845b-1e978e5a6942</t>
+          <t>3e341bc9-6ebe-4f61-93f0-7ee6679e542f</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>232c7a99-3f0f-4141-8ade-e62f28d4e618</t>
+          <t>3f33b058-4c72-403e-995b-23dc23b7bcbd</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>23d2803a-4904-443d-abc4-569bd54e7f89</t>
+          <t>3f5ea3a2-ffb9-475f-867a-67bd99f8833f</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>24ff293b-21a0-44c9-85a2-1b5c3aa5fdb2</t>
+          <t>3fab2a04-af5e-409f-a0fb-24f0dbb9e6be</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>250648a0-1984-4747-ae8f-ccd2152fbf77</t>
+          <t>40920589-eb88-464d-85b5-c1971b26ece6</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>25a2808d-d12e-4c4c-9aba-c2e83b0eb6f6</t>
+          <t>40bc05cd-ce59-4801-92db-ca89b6d2920e</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>267ffbe9-98c3-4330-b6ad-6c73e89e8688</t>
+          <t>41edce86-9f73-45a7-b38e-ba23cc0822cd</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>28bedf49-ef8d-40ad-84e7-c3cf6e3c5d44</t>
+          <t>445e1399-d5d1-4a8f-8a8a-f02cf5f6849a</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2bdf89b5-e24d-4cb7-a664-62d1e93e631c</t>
+          <t>44a83362-0b4a-425d-b735-e56dd8924aad</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2c33a6af-c9d9-49a4-9729-ccf42f2305db</t>
+          <t>463ea11e-a23c-4c26-95d2-4207ae5c1ea3</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2e182896-19c4-4d6e-a239-4b76b5ad5c75</t>
+          <t>4c85e03f-631a-4227-96ff-e6c4c9108707</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2eff83d6-b12d-4bb6-9ee4-1c79e46e96e4</t>
+          <t>4ed7119a-c5d2-4081-8056-400f7267b81d</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>309eae22-2930-4315-9409-203a4ab1786f</t>
+          <t>517cfff5-6f3f-4ee1-96eb-bb07e8c289fc</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>311030c7-6916-4ca5-9c56-a9239953dcb2</t>
+          <t>53d433c0-17d1-42e1-8a01-2959ce73e3cf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3141db17-b19c-41fb-9cc2-d37651f4d7a1</t>
+          <t>54fffd1e-283a-46d5-908d-aae8c76d04e9</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>330a7779-593a-4384-ac36-d6d2f6f4b3ee</t>
+          <t>558e9353-f4f4-4097-a40c-599fa1ce86cd</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>33656252-a79c-4e52-be79-4062a743a718</t>
+          <t>56cf1672-11d6-413a-b8e8-569894f48847</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>343d3602-bb26-4e35-99d4-830d616ca923</t>
+          <t>5a295b38-58ac-492d-8ef1-e2b8d458a4c0</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>37decbe4-09d2-41a7-9f74-436405beec3a</t>
+          <t>5bd3e912-408d-4a6c-ae70-34fc996937a0</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>3837e5c8-d65e-472e-8d8c-860d81a22c38</t>
+          <t>5c7866aa-e643-414c-be29-bcae2f0a9ee7</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>38a6c369-98e6-4a93-ab73-461dc73c33f5</t>
+          <t>5d2ce8b8-da0f-4fea-ba61-6477178ddafd</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>3a4feed5-e8e6-416a-81aa-9a675bf3fc56</t>
+          <t>5d63fdec-c5fb-41e5-a6b8-cc90e93090c3</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3bcf62e5-1b79-484b-bf47-fb8f4b5c3d63</t>
+          <t>5d67a2bb-dbc1-43c5-a3e3-62a63df16527</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>3f9e08c3-7cc5-42b4-b761-ba9187d5c067</t>
+          <t>5dccd7c8-069e-4848-913a-305d112fec83</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>40e2a600-0690-4537-a229-a7c367e89618</t>
+          <t>5e30be7a-f6df-474f-8d8e-f6c6e54b1f04</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>435411e7-bde7-4991-a8db-c02fbb3fec55</t>
+          <t>606edfc9-1ce1-421a-aa34-b220e74808cb</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>43d82037-ee10-439d-a12b-531db07715b7</t>
+          <t>62d8494e-7b06-45b6-a483-9ea0af00396c</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>441d1efa-b458-44b1-aece-3fac457823fe</t>
+          <t>63422d2d-1762-4194-8e16-34df0a27a4dc</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>4718233f-4cdc-42bd-affb-6f247c560239</t>
+          <t>63802b89-59c9-4e00-984c-1cb374671ba6</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>494f8c3a-be47-46e5-83ed-3c6c0f71b79c</t>
+          <t>69162a01-e6af-42b7-b4b6-73e852232b9d</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>495a3268-c3e0-49b7-865f-34868335258a</t>
+          <t>6995a682-e65f-412e-9e8d-a80390a9c02d</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>4b44783c-a75d-4d87-bc0b-960615c10a84</t>
+          <t>6bba76db-dd14-466b-be1c-e0e22095e50f</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>4b9832f9-fb46-48a4-9d07-1a75fe0eb75e</t>
+          <t>6c30823c-6fb8-4391-a0ff-be152bf4e43a</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>4bb43afb-1e2b-45d9-bba8-9ba7def45b26</t>
+          <t>6c66e409-233d-446e-91ee-7bf9c22f72fe</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>4bd64886-1d7f-4a2d-8fc2-035790dce037</t>
+          <t>701c8dd3-1d33-4da6-ac70-63d135edfde0</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>4cf90c1b-0df0-4d70-b2e7-4f8f68bac7e2</t>
+          <t>77f70e54-b088-4195-8ca8-a8c9b22a87a8</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>4d4c9e59-5ed4-463f-a14a-ce0d0af0725d</t>
+          <t>77f7aad3-dd8c-4ead-b9e5-e61d953c2e8f</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>4e11d282-3060-4213-af75-070a210c32e7</t>
+          <t>78da614e-1baf-4b35-a682-68d7d35d43ea</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>4f5ac3ce-547c-4995-8f86-443aecdc841b</t>
+          <t>7b1bd4f5-0157-4cf1-8335-ba5513c3e05b</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>4f7923de-94ce-4a76-a38d-5ccaaab7c7b1</t>
+          <t>7c97c385-96a5-4bde-9886-8857ba434cea</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>52e94329-21bc-4357-985c-64ba9f1be818</t>
+          <t>7d1c1338-6436-426d-8db2-452954c73ae4</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>534ecc3c-de55-4149-a15d-030c042ba8af</t>
+          <t>7e31fe93-2716-41a0-85c7-79b69ca58241</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>5655a36e-eb1b-4f2e-bac3-c8d3f80b4c23</t>
+          <t>7e37939d-7d58-4c46-8535-12d6fecfc48c</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>56f0d7e0-70f0-45d6-a708-ee332c9602a3</t>
+          <t>7eda8ca8-774d-422a-be49-6c623b18c081</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>5743bec6-6a64-409f-bee1-9f190c4a38a3</t>
+          <t>80c4d787-1992-4bec-b421-124f48bdec32</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>575edd2c-088e-4fce-8d34-c0f54efb0225</t>
+          <t>80fd0fdc-0613-4fb9-963d-787361346999</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>57ebe591-3de0-4518-9148-ca14bdf2c9e7</t>
+          <t>81be1be8-02df-4e0a-bee7-a90332035589</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>5913e5b3-31b4-4962-918f-6acc50ba1665</t>
+          <t>845d4c1e-3c7c-40b0-ad75-6e43377c2c5d</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>5b68f417-a54a-492d-81c9-32594b83fb23</t>
+          <t>845dfa8d-1bba-4be2-b7db-54d49505815c</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>5c8f0100-6d55-4bce-b6d0-f792268ec35e</t>
+          <t>867ff8f9-df50-40c4-a972-d7e6bfe889e4</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>5cc9f808-1e70-4de0-a0d9-4180ee28b7be</t>
+          <t>89b0f74b-fb80-429c-a9ab-a8f8d33b525e</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>5f77b8ac-fbdc-4c7a-b73e-29b584d5e00a</t>
+          <t>8a7ae572-5801-499b-b1c7-73434ddb396f</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>630224d5-61e6-4c7e-9c1c-110e5d369422</t>
+          <t>8b0f7864-4388-4a89-bcaa-0ac112273085</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>63242424-87ed-4063-8fc2-8ff12b55fc49</t>
+          <t>8b124131-f749-42ac-9d27-692474f53a64</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>64f5bf96-09d2-4f24-b3cf-fa83700604d9</t>
+          <t>8d33e09b-50e9-4e16-a4d5-9602b7328ce8</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>659073d6-2acd-4181-80cd-b0e076c0fea0</t>
+          <t>8d78a7dc-688b-4446-82da-0935b871aa5f</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>679118f5-c1d7-4342-9515-2f332be04cea</t>
+          <t>8ee56e9a-00c0-4522-aefd-55c7556a5d30</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>699875e9-bade-4bb1-9f6f-fd3025abfd46</t>
+          <t>942e220d-a44b-414e-bfed-8d77feedaba4</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>6a937c60-399e-4835-837c-973cebca448e</t>
+          <t>95068c2c-e61b-43f0-9f18-38a97e5bc914</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>6b8d3b0a-eb85-4fc5-9c62-5c447da99442</t>
+          <t>96928b20-8815-4a43-bc36-9f17ebcf1d42</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>6d47b10b-c961-4f28-91f1-b4b5726cdaf2</t>
+          <t>96c9f5bf-145a-48b1-9dbd-aaf6427284e8</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>6daf2bcf-7c8f-43ec-8c44-dd903a8d9a53</t>
+          <t>98c58b22-9a46-40ee-9c9b-808d4636c35c</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>72491ff3-5886-4a91-90ca-b54d15ef3c3e</t>
+          <t>99b73b82-9e03-4228-80c4-dae7d5854713</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>72834bef-3d98-464b-b379-8f17571b52f2</t>
+          <t>9a109b0f-aa49-4ef1-a335-12288cda0bab</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>72c4408a-dacf-4164-a66a-1253869ab814</t>
+          <t>9a43a9ae-d6ae-4c4f-9459-18ba06026cf9</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>7363506f-8d0e-4b57-9a61-8bb7a176ae33</t>
+          <t>9c74e2ad-75b6-4a0f-8da8-38c0c4f484cc</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>73c3d7ad-1952-4025-a5ff-6e100343673a</t>
+          <t>9d4907f0-71ab-40e0-b1a4-11e01b237e80</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>74e09cc2-c07d-417d-ac27-79d1ad164c19</t>
+          <t>a019126f-1c64-4bbd-8e90-0f0564526625</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>75317cfb-bd20-4744-bc5e-0ee95ac27ba3</t>
+          <t>a1d3a9d4-eef3-4599-bd9f-5529ec8d3690</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>75e57185-589a-4640-94d3-4b84e7143c9d</t>
+          <t>a22831d2-d0ef-4d29-92ec-e4a0db07b9ef</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>76d76f26-c221-4e5c-aac7-d03383991dcc</t>
+          <t>a234b282-98e1-44f8-9fbf-d008ea46aaf7</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>7707c4dc-be69-4176-aad7-fbd2492c12ec</t>
+          <t>a5760656-1cf5-4e4b-9e1a-937bc751fb4a</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>790ed31d-8b70-4d37-9b92-5074047016d1</t>
+          <t>a6e9361c-6272-489e-a58e-195924fe1c20</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>7a4941db-606e-4586-a7b6-e0489d3b39ce</t>
+          <t>aad2bc49-d858-4522-96b1-bddeeb09bd60</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>7af43e66-8a47-4381-a06a-336a8ae876fe</t>
+          <t>ab18f839-acbd-4494-bfa0-e613b10ae637</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>7b983f17-8474-4488-b566-b88dd8652246</t>
+          <t>adee03d2-cff8-4818-a5c4-39d6bf02ef00</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>7bba7aee-2684-4652-9634-3eb15196dadb</t>
+          <t>af424e9e-080d-48c1-9206-8389afa2bce6</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>7bd4e0ac-0096-4833-a5a2-5f383efeabc8</t>
+          <t>b23e3495-8c43-4380-8908-1038f220c673</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>7dc8d41d-bc2d-4b8d-9d12-8380d4b2dea0</t>
+          <t>b3b8b2e3-bb23-4950-bb73-5d61136a8b18</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>7ec1fbfc-4263-4a1b-bf84-1492dc1f4afa</t>
+          <t>b5487ba5-9c9a-4c02-86a6-df20854db6a8</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>7f17e2b1-5e3c-4994-a37d-c74a50714df1</t>
+          <t>b757e203-3856-40dd-8395-a307b74b1fc6</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>8038f84f-a209-4d61-8e2c-32e323341f47</t>
+          <t>b874510a-ff42-4ecf-8b67-0307e0d4a533</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>82532323-ffca-48a6-88c2-45f727a96a41</t>
+          <t>be062360-8524-4a15-87b3-50af2ec7e51f</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>82ca4eed-fa30-4a37-a1bb-77de95e997bb</t>
+          <t>be7363a7-7770-464d-bbb1-7d7d086a4714</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>857eef3d-eaaf-480a-aac3-4f1e030a4918</t>
+          <t>beadf9fb-d1e2-4868-a15d-6c0c15af93df</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>87dd938f-1604-4393-8e15-981c461b9b42</t>
+          <t>c3cc9f40-7664-48dd-a34a-2bc18c669bef</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>88268daa-2d70-45f4-94fc-355e12143ad9</t>
+          <t>c70d09c0-b75d-4146-86d4-e9519d800151</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>88c997e3-44ef-4fb3-83de-b6d7e3e54a47</t>
+          <t>c730575a-d4f5-453e-ba5e-4d4874d14b62</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>8a79faec-44a9-4aff-ba23-164f394ce655</t>
+          <t>c78b0c19-849e-4d80-87e4-e1f671466f71</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>8c4e4a92-7d26-40ca-b7ff-a85a58fc5cdb</t>
+          <t>c7ecf24e-3233-45d9-97d7-26c09f87b297</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>8de93702-e6dc-40b0-8fb1-dcf9a9712ad2</t>
+          <t>c9a6ac1b-50d8-4afb-8a59-44a742f6b0a2</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>8eab5521-7a5a-416b-870c-2bc2971224d2</t>
+          <t>ca1e344e-7e6b-49ca-b39b-cf51f29bc9b0</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>8fc0c7f8-8489-4ea9-a358-c159b17a72ca</t>
+          <t>ca9378c0-9d7a-47be-bac2-27214890723b</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>9081da4c-cd92-42e2-9a57-b4e780e0e126</t>
+          <t>cc0e653b-aceb-4cb7-816a-c3a85f9da6aa</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>914c7f0d-6fe5-4a2b-959c-aae3fe58052a</t>
+          <t>d1b09fc7-731a-457f-aae1-8f7c2ea128f0</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>92a7ea6e-bdd8-4d82-8bfb-3c960f5c2d1c</t>
+          <t>d3dfd9b6-0514-41e2-81e7-df970fb254ff</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>949077f3-5b09-4aec-b1b9-23a27fe7b57b</t>
+          <t>d7120451-8526-471e-8e5a-654124917299</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>96ee4c4b-cc58-4f83-a2e8-96b728327bfe</t>
+          <t>da68508a-b84e-47d7-8e0b-8aefc4760ed5</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>9894f3ba-930d-466c-96f3-396d897366a8</t>
+          <t>db8bd60f-9171-4027-8054-4a753cc28e5e</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>9bb74bc7-64e1-4abe-84fb-c801cbdebf0e</t>
+          <t>dcaf9267-7b55-4df7-b464-d8e281a9256c</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>9e856590-a2e2-404d-ba49-68f1a843d40f</t>
+          <t>de78c7a0-1b21-451b-80b1-6da4cd24bc8d</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>9efed40c-8f03-4a33-8190-7439bd611b21</t>
+          <t>dea006cf-e597-4171-b382-09470b0a1633</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>9fd4c57e-e279-4860-81a5-f47956e37641</t>
+          <t>def4c5f2-1c6c-474a-ba28-f5408540606d</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>a0dd4d8c-c7e5-4ba8-a655-daaf6f77f714</t>
+          <t>df1a8e05-27c4-4c81-99af-8bc0eb424f30</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>a0f2f1ff-4c5d-4954-856e-23daf6622152</t>
+          <t>e0cd89c0-b625-47f9-9f6a-392063bc6969</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>a651ba03-9280-4ff0-8d64-71426f4919d7</t>
+          <t>e17e7b5f-d236-47ff-a28f-ff514dbe894b</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>a6d37145-5b15-4661-a714-a9cc9e20badc</t>
+          <t>e2947e2a-4673-4145-bd55-474424e68f31</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>a91ed672-9431-4389-bb11-8125b30a3629</t>
+          <t>e2b1cbac-b1e9-48b6-b96f-32e37a4d1aeb</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>a9973184-606f-4801-9da1-a998e0c27437</t>
+          <t>e45cb59f-88ea-4f0d-a2f9-b6118e5e6745</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>aad9a154-3e75-4cc0-8d71-b73c96ac83db</t>
+          <t>e4914d0a-7172-4dae-8379-9f19497986e6</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>ac6505bd-63d0-4504-8417-463149a4239a</t>
+          <t>e660b3f4-4f7a-42e8-b985-0b61a2d58901</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>ad77f21b-b0b4-420f-9a7c-2f17d14a7ae9</t>
+          <t>e772e7d7-4593-4366-b233-4c9d8cd9cc9a</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>ada7b268-9138-4fb6-91fe-e38822acdb37</t>
+          <t>ea61fe3a-4501-406b-9906-43fb82845a58</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>ae45bfe2-f70c-47fc-8f3e-5899eecdf4ba</t>
+          <t>ee9531d6-5b66-4c35-8ab8-96c553b71447</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>b0ada692-ad10-4454-ac73-a1321659d2aa</t>
+          <t>ef1c3fb9-4ed1-47af-8de3-431cf8dc581c</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>b1d33fb6-8964-4138-9d67-f158866a5a81</t>
+          <t>efe22036-611c-4001-b1fc-a7aacd159417</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>b6b2a641-fa11-4566-a7e6-83093e10c6a6</t>
+          <t>f25c2106-5f46-478a-a58f-faa693324613</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>b9fd443d-a097-4aaf-ba14-9629d7eb83dc</t>
+          <t>f2e7d36e-7067-4c41-836c-bef2fa0befeb</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>be5b6fc1-458d-420a-bf19-0caaf4080f81</t>
+          <t>f3b47ef1-306b-4ecd-b740-72324bb8fa15</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>be6886ec-3f52-4baf-b5c6-82093855e634</t>
+          <t>f3e4cdd4-1909-42d1-91b1-ceeb0a42c9f9</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>bfd8eb6a-6214-499d-93d8-8c1f8ea6ac33</t>
+          <t>f411c1d3-5df8-4a1e-ac30-40cdb0ccafb1</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>c00402c1-c4ce-49da-81c8-e94952d6b43e</t>
+          <t>f4b02cd3-7893-41e7-bcda-5d6bc0036a07</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>c17806dc-a63f-4a6e-9826-7f0faa4c1f48</t>
+          <t>f5622aba-348f-43e0-8a10-2ed65ae2b912</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>c3d1140d-bc28-4fe9-bb59-2facb6fd5775</t>
+          <t>f5efd8ee-5d4a-4f22-b229-9ab4c2bc9976</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>c71e50e1-46de-4882-8cc7-b819b63323cd</t>
+          <t>f730721f-f37d-446a-986c-d97131afbd62</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>c83737d1-6102-4e82-aa58-8ff103434406</t>
+          <t>f861b94e-f4df-4a80-a1ab-2ba97c4a01b8</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>c85c25db-089a-42f2-a2ef-85b3a05dea1b</t>
+          <t>fb893d1f-9cbb-4118-86b5-574d6bab278d</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>cb387d4e-c8ff-4e40-b16e-55e1109860cd</t>
+          <t>fbc9606b-ce87-44bb-acff-b36d26a129f9</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>cc9e1850-c418-4891-8cce-635413d0c31f</t>
+          <t>fd4dc726-c4e3-428f-8b8e-7eefd50fb095</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>cd10c05a-5b03-4aa4-9734-184b7cfb5836</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>cd339ffb-9dc9-466d-9b2a-503891a9a684</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>cde51c1b-ee66-4cc1-9504-27c0e37375aa</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>cee638ae-4724-4607-ba48-d964b02efcdc</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>cfebab11-31b5-4bb9-828e-b250c3bfcdad</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>d2fd8b9b-9ec4-49cb-af50-750977f4d5e3</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>d56ac28e-7d94-462d-91ea-8df80985fe25</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>d5e330ba-7a27-4511-8af9-3d31ebf054dc</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>d63012fe-c707-4a3b-9bd5-ca321afb1457</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>d734b494-b066-4244-9754-108071829e70</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>d82d9002-5ca9-4379-b1b7-d87953939e70</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>d871bcf0-a654-4d7e-a291-42f461a9a5f5</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>d8c93311-a9e4-464e-a9ac-3802ac413363</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>d912bb5e-f260-4cda-b1a9-d20842e4e5af</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>dc6b1120-b3c2-4e43-99bb-998405f25bbd</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>dfe24cba-a1f9-4152-90bb-41688969e5ec</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>dff83532-84fd-4267-a269-3a469fbae37a</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>e045dac3-5af4-4a4a-afb6-1f38eda7daee</t>
-        </is>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>e3eb24ef-43a5-4c6d-b98f-6cd0dc314a67</t>
-        </is>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>e5701635-0e00-4da8-ab33-0883d4bf32eb</t>
-        </is>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>e5ee68f4-a9ef-44b3-95d2-d22b1699ff62</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>e61d98bf-7bed-45b7-8f8f-be5e212705a6</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>e6d33331-5d43-4594-97e5-9ef7dadc26c2</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>e736145b-7040-434d-a3b3-834d0a658adb</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>e7f54243-6313-427b-91dc-f5570b0d1011</t>
-        </is>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>e8216a04-e550-460f-84c9-830b0933f16e</t>
-        </is>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>e9a79c76-51d5-4fe2-a0c3-8c1d227178a7</t>
-        </is>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
-        <is>
-          <t>eaad3797-8001-429c-a1f8-8136741079dc</t>
-        </is>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
-        <is>
-          <t>ebf82e35-f67e-4575-8c09-9b62298dcd21</t>
-        </is>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
-        <is>
-          <t>ec772f9c-f6a7-4545-aa86-09e6ebf2c506</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>eccb51da-8abb-4e4c-8b3b-bb841adb4363</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>ecf26a0a-20f7-4048-9954-c0dddc58ec9a</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>ee5822be-c3e1-44f3-b363-b4f78a15a41f</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>ee8e7970-43af-479b-90ad-1c2e5f626b65</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>ef174c1d-a179-4e6c-9be4-c0cd02245e4c</t>
-        </is>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>efc5c64d-b4fc-4999-ab53-92efc19dc278</t>
-        </is>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>f1994467-e982-4e9f-8ae3-aedfb8c81b55</t>
-        </is>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>f33e1702-ba18-421c-a2dc-6af5f3bb98ca</t>
-        </is>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>f37ab4d9-043f-4aa7-93fe-b0d06ef4c2ce</t>
-        </is>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>fa399a66-4f5d-4d59-bc0d-35c3780f9e0c</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>fb0a55c5-d40c-47a2-b1b7-250b9b376a3b</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>fb3e6cf9-fe94-4434-b443-4f3ebf75e3e7</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>fbd52bbc-8c87-478a-88a7-8349f9bc755a</t>
-        </is>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>fd521002-ee1e-4700-8c25-458d3aa125b5</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>fff785ef-d17c-49a9-b808-291b987ea9da</t>
+          <t>fee8716c-c950-4056-9947-799ad31a39e2</t>
         </is>
       </c>
     </row>

</xml_diff>